<commit_message>
Tp Gestione Ente Caricato in TFS
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0/NR 28.05.22/tp gestione ente.xlsx
+++ b/docs/tp/Sfera_4.0/NR 28.05.22/tp gestione ente.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Sfera_4.0\NR 28.05.22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F3CEF7-1198-4A82-96DE-E363230F0CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D07F06-F932-47AE-B4F2-8C3B6A0CBFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="255" windowWidth="19440" windowHeight="15000" xr2:uid="{4E8894D9-71E2-4277-A4DD-41C2ED1226B1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8894D9-71E2-4277-A4DD-41C2ED1226B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>Sfera 4.0 - Operatività - STAMPA AVVISI - Gestione Stampa avvisi modalità massiva_gestione ente _parametri di default associati alla vista</t>
   </si>
   <si>
-    <t>verificare che avendo selezionato la voce gestione ente,risultano selezionati di default i seguenti parametri:-Agenzie/ Fonti selezionate: tutte le agenzie relative alla Compagnia 73 (LLoyd); le agenzie relative a Compagnie diverse dalla 73 dovranno risultare sabbiate e non selezionabili;-LoB selezionate: tutte;-Periodo di competenza: mese successivo a quello corrente (t+1). L’utente può selezionare un dei due mesi solari disponibili per questa vista, t+1 che sarà impostato di default oppure t+2. Se l’utente modificare il periodo di competenza, deve cliccare sul componente della “Data Inizio”, che si imposterà in automatico sul primo giorno del mese selezionato, mentre la “Data Fine” si imposterà in automatico sull’ultimo giorno del mese;-Stati selezionati: In lavorazione, Da lavorare. Questi sono gli unici stati disponibili in questa vista-Nessun cluster selezionato.</t>
-  </si>
-  <si>
     <t>Sfera 4.0 - Operatività - STAMPA AVVISI - Gestione Stampa avvisi modalità massiva_gestione ente_colonna ente di genarazione avvisi</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Sfera</t>
+  </si>
+  <si>
+    <t>verificare che avendo selezionato la voce gestione ente,risultano selezionati di default i seguenti parametri:-Agenzie/ Fonti selezionate: tutte le agenzie relative alla Compagnia 73 (LLoyd); le agenzie relative a Compagnie diverse dalla 73 dovranno risultare sabbiate e non selezionabili;-LoB selezionate: tutte;-Periodo di competenza: mese successivo a quello corrente (t+1). L’utente può selezionare un dei due mesi solari disponibili per questa vista, t+1 che sarà impostato di default oppure t+2. Se l’utente modificare il periodo di competenza, deve cliccare sul componente della “Data Inizio”, che si impostearà in automatico sul primo giorno del mese selezionato, mentre la “Data Fine” si imposterà in automatico sull’ultimo giorno del mese;-Stati selezionati: In lavorazione, Da lavorare. Questi sono gli unici stati disponibili in questa vista-Nessun cluster selezionato.</t>
   </si>
 </sst>
 </file>
@@ -220,7 +220,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +236,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -283,6 +289,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -599,22 +612,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4144F51-E05B-4F34-8726-0B68B5F02E89}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31.26953125" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="31" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -641,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>12295</v>
       </c>
@@ -660,13 +673,13 @@
         <v>10</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
@@ -681,7 +694,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="5" t="s">
         <v>14</v>
@@ -698,13 +711,13 @@
         <v>10</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="50" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -719,7 +732,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="5" t="s">
         <v>16</v>
@@ -736,13 +749,13 @@
         <v>10</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="50" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
@@ -757,11 +770,11 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" ht="344.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="312.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>13</v>
@@ -772,10 +785,10 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
@@ -789,17 +802,17 @@
         <v>10</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="50" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>13</v>
@@ -810,435 +823,502 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="6" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:9" ht="100" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="50" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="100" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="125" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="255" x14ac:dyDescent="0.2">
-      <c r="C22" s="3" t="s">
+    </row>
+    <row r="23" spans="2:9" s="6" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="2:9" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" s="6" customFormat="1" ht="50" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="2:9" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="4">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" s="6" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="2:9" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" s="6" customFormat="1" ht="50" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="2:9" s="6" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="4">
+        <v>2</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" s="6" customFormat="1" ht="50" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="2:9" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="8">
+        <v>2</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" s="9" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="1">
-        <v>2</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="2:9" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="5"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="1">
-        <v>2</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="2:9" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="5"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="4">
+        <v>2</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" s="6" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="1">
-        <v>2</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B39" s="3" t="s">
+      <c r="E39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="C40" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="1">
-        <v>2</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="137.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="B41" s="3" t="s">
+      <c r="E41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" t="s">
+        <v>53</v>
+      </c>
+      <c r="I41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="1">
-        <v>2</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" t="s">
-        <v>54</v>
-      </c>
-      <c r="I41" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B43" s="3" t="s">
+      <c r="E43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" t="s">
+        <v>53</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="1">
-        <v>2</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H43" t="s">
-        <v>54</v>
-      </c>
-      <c r="I43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="C44" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>

</xml_diff>